<commit_message>
Fixed modelling with simplified plug.
</commit_message>
<xml_diff>
--- a/example/info/02 processed info.xlsx
+++ b/example/info/02 processed info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S101"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>test id</t>
+          <t>test_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>old filename</t>
+          <t>old_filename</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>test type</t>
+          <t>test_type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>A_0 (mm)</t>
+          <t>A_0_(mm)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>h_0 (mm)</t>
+          <t>h_0_(mm)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>foot correction</t>
+          <t>foot_correction</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
@@ -527,6 +527,16 @@
       <c r="S1" s="1" t="inlineStr">
         <is>
           <t>YP_0.002_1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>UTS_0</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>UTS_1</t>
         </is>
       </c>
     </row>
@@ -590,15 +600,17 @@
       <c r="Q2" t="n">
         <v>0.000343613133393793</v>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>[0.00595534]</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>[251.96596728]</t>
-        </is>
+      <c r="R2" t="n">
+        <v>0.005955339826859217</v>
+      </c>
+      <c r="S2" t="n">
+        <v>251.965967279652</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.07539615443422459</v>
+      </c>
+      <c r="U2" t="n">
+        <v>277.080919182671</v>
       </c>
     </row>
     <row r="3">
@@ -661,15 +673,17 @@
       <c r="Q3" t="n">
         <v>0.0004895812404323431</v>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>[0.00665334]</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>[252.88748701]</t>
-        </is>
+      <c r="R3" t="n">
+        <v>0.006653338845315306</v>
+      </c>
+      <c r="S3" t="n">
+        <v>252.8874870084364</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.07875696706349665</v>
+      </c>
+      <c r="U3" t="n">
+        <v>277.834142238505</v>
       </c>
     </row>
     <row r="4">
@@ -732,15 +746,17 @@
       <c r="Q4" t="n">
         <v>0.000530764702328129</v>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>[0.00589268]</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>[254.02447229]</t>
-        </is>
+      <c r="R4" t="n">
+        <v>0.005892677469428021</v>
+      </c>
+      <c r="S4" t="n">
+        <v>254.0244722851376</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.07814439258086513</v>
+      </c>
+      <c r="U4" t="n">
+        <v>280.209188306993</v>
       </c>
     </row>
     <row r="5">
@@ -803,15 +819,17 @@
       <c r="Q5" t="n">
         <v>9.183978673318427e-05</v>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>[0.00540802]</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>[239.82784953]</t>
-        </is>
+      <c r="R5" t="n">
+        <v>0.005408015414077331</v>
+      </c>
+      <c r="S5" t="n">
+        <v>239.8278495292511</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.06707426910420559</v>
+      </c>
+      <c r="U5" t="n">
+        <v>265.627730964216</v>
       </c>
     </row>
     <row r="6">
@@ -857,13 +875,13 @@
         <v>192.947593520996</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0005903185807671863</v>
+        <v>0.0005903185807671859</v>
       </c>
       <c r="M6" t="n">
         <v>35.2190159803605</v>
       </c>
       <c r="N6" t="n">
-        <v>59661.03241166723</v>
+        <v>59661.03241166724</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -872,17 +890,19 @@
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
-        <v>-0.0004346933673407137</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>[0.0060991]</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>[244.5562676]</t>
-        </is>
+        <v>-0.0004346933673407142</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.006099095468387027</v>
+      </c>
+      <c r="S6" t="n">
+        <v>244.5562675979567</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.07748823857970359</v>
+      </c>
+      <c r="U6" t="n">
+        <v>273.200295913472</v>
       </c>
     </row>
     <row r="7">
@@ -945,15 +965,17 @@
       <c r="Q7" t="n">
         <v>0.0003567081833944904</v>
       </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>[0.00630495]</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>[239.7774238]</t>
-        </is>
+      <c r="R7" t="n">
+        <v>0.006304948317891945</v>
+      </c>
+      <c r="S7" t="n">
+        <v>239.7774237994842</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.07394407507141819</v>
+      </c>
+      <c r="U7" t="n">
+        <v>267.412779741201</v>
       </c>
     </row>
     <row r="8">
@@ -1016,15 +1038,17 @@
       <c r="Q8" t="n">
         <v>0.0001712096225899404</v>
       </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>[0.00651891]</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>[279.67343248]</t>
-        </is>
+      <c r="R8" t="n">
+        <v>0.00651890866018981</v>
+      </c>
+      <c r="S8" t="n">
+        <v>279.6734324776601</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.09270740042560785</v>
+      </c>
+      <c r="U8" t="n">
+        <v>308.906990845537</v>
       </c>
     </row>
     <row r="9">
@@ -1087,15 +1111,17 @@
       <c r="Q9" t="n">
         <v>0.0004134955762651457</v>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>[0.00662082]</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>[267.42109477]</t>
-        </is>
+      <c r="R9" t="n">
+        <v>0.00662081759751331</v>
+      </c>
+      <c r="S9" t="n">
+        <v>267.421094767428</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.1130343672647691</v>
+      </c>
+      <c r="U9" t="n">
+        <v>300.687648326774</v>
       </c>
     </row>
     <row r="10">
@@ -1158,15 +1184,17 @@
       <c r="Q10" t="n">
         <v>-0.0004316940708122634</v>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>[0.00687551]</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>[264.47172192]</t>
-        </is>
+      <c r="R10" t="n">
+        <v>0.006875505241530501</v>
+      </c>
+      <c r="S10" t="n">
+        <v>264.4717219167996</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.05986655723622183</v>
+      </c>
+      <c r="U10" t="n">
+        <v>292.441626898986</v>
       </c>
     </row>
     <row r="11">
@@ -1229,15 +1257,17 @@
       <c r="Q11" t="n">
         <v>-0.0002246542070388807</v>
       </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>[0.00635436]</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>[253.15240602]</t>
-        </is>
+      <c r="R11" t="n">
+        <v>0.006354360819481954</v>
+      </c>
+      <c r="S11" t="n">
+        <v>253.1524060217465</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.07899122785625572</v>
+      </c>
+      <c r="U11" t="n">
+        <v>285.69504833639</v>
       </c>
     </row>
     <row r="12">
@@ -1300,15 +1330,17 @@
       <c r="Q12" t="n">
         <v>0.0008862018816846342</v>
       </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>[0.00692006]</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>[258.26045203]</t>
-        </is>
+      <c r="R12" t="n">
+        <v>0.006920060520437712</v>
+      </c>
+      <c r="S12" t="n">
+        <v>258.2604520284232</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.08743702618949672</v>
+      </c>
+      <c r="U12" t="n">
+        <v>291.821443265679</v>
       </c>
     </row>
     <row r="13">
@@ -1371,15 +1403,17 @@
       <c r="Q13" t="n">
         <v>0.0002462890752533788</v>
       </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>[0.00656171]</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>[248.91961011]</t>
-        </is>
+      <c r="R13" t="n">
+        <v>0.00656171146327205</v>
+      </c>
+      <c r="S13" t="n">
+        <v>248.9196101116396</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.09356067858824338</v>
+      </c>
+      <c r="U13" t="n">
+        <v>282.622139614456</v>
       </c>
     </row>
     <row r="14">
@@ -1442,15 +1476,17 @@
       <c r="Q14" t="n">
         <v>0.0003095039103118984</v>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>[0.00631948]</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>[248.3971272]</t>
-        </is>
+      <c r="R14" t="n">
+        <v>0.006319480966726892</v>
+      </c>
+      <c r="S14" t="n">
+        <v>248.3971271986643</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0832295080824403</v>
+      </c>
+      <c r="U14" t="n">
+        <v>276.607824736583</v>
       </c>
     </row>
     <row r="15">
@@ -1513,15 +1549,17 @@
       <c r="Q15" t="n">
         <v>0.0001167273405350824</v>
       </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>[0.00618976]</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>[245.73442059]</t>
-        </is>
+      <c r="R15" t="n">
+        <v>0.00618975878531404</v>
+      </c>
+      <c r="S15" t="n">
+        <v>245.7344205904582</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.08975918584984638</v>
+      </c>
+      <c r="U15" t="n">
+        <v>276.35304034072</v>
       </c>
     </row>
     <row r="16">
@@ -1584,15 +1622,17 @@
       <c r="Q16" t="n">
         <v>9.531691839774926e-05</v>
       </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>[0.00527041]</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>[240.67871789]</t>
-        </is>
+      <c r="R16" t="n">
+        <v>0.005270409387028891</v>
+      </c>
+      <c r="S16" t="n">
+        <v>240.6787178901594</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.09074228584900475</v>
+      </c>
+      <c r="U16" t="n">
+        <v>274.610658491</v>
       </c>
     </row>
     <row r="17">
@@ -1655,15 +1695,17 @@
       <c r="Q17" t="n">
         <v>-0.0001668037782862342</v>
       </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>[0.007061]</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>[303.28881334]</t>
-        </is>
+      <c r="R17" t="n">
+        <v>0.007060996000749431</v>
+      </c>
+      <c r="S17" t="n">
+        <v>303.2888133397277</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.07904338585557306</v>
+      </c>
+      <c r="U17" t="n">
+        <v>331.306057883049</v>
       </c>
     </row>
     <row r="18">
@@ -1726,15 +1768,17 @@
       <c r="Q18" t="n">
         <v>0.0004536535710335157</v>
       </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>[0.00767737]</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>[283.10466726]</t>
-        </is>
+      <c r="R18" t="n">
+        <v>0.007677373993186945</v>
+      </c>
+      <c r="S18" t="n">
+        <v>283.1046672576235</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.09452658219299272</v>
+      </c>
+      <c r="U18" t="n">
+        <v>304.743333329536</v>
       </c>
     </row>
     <row r="19">
@@ -1797,15 +1841,17 @@
       <c r="Q19" t="n">
         <v>-0.0005549399286298978</v>
       </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>[0.00686329]</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>[274.69125295]</t>
-        </is>
+      <c r="R19" t="n">
+        <v>0.006863290910295042</v>
+      </c>
+      <c r="S19" t="n">
+        <v>274.6912529499168</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0701139263847103</v>
+      </c>
+      <c r="U19" t="n">
+        <v>319.747323675888</v>
       </c>
     </row>
     <row r="20">
@@ -1868,15 +1914,17 @@
       <c r="Q20" t="n">
         <v>-0.0004259274742736629</v>
       </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>[0.00587294]</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>[267.7587454]</t>
-        </is>
+      <c r="R20" t="n">
+        <v>0.005872942843778696</v>
+      </c>
+      <c r="S20" t="n">
+        <v>267.7587453982311</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.08178154082245984</v>
+      </c>
+      <c r="U20" t="n">
+        <v>289.881300173436</v>
       </c>
     </row>
     <row r="21">
@@ -1939,15 +1987,17 @@
       <c r="Q21" t="n">
         <v>-8.019852286719363e-05</v>
       </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>[0.00602558]</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>[240.21867153]</t>
-        </is>
+      <c r="R21" t="n">
+        <v>0.006025575179708148</v>
+      </c>
+      <c r="S21" t="n">
+        <v>240.2186715339491</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.05968749180149951</v>
+      </c>
+      <c r="U21" t="n">
+        <v>252.998046400138</v>
       </c>
     </row>
     <row r="22">
@@ -2010,15 +2060,17 @@
       <c r="Q22" t="n">
         <v>9.097191051991339e-05</v>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>[0.0055403]</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>[205.94052989]</t>
-        </is>
+      <c r="R22" t="n">
+        <v>0.005540301663927031</v>
+      </c>
+      <c r="S22" t="n">
+        <v>205.9405298924263</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.04688409558147731</v>
+      </c>
+      <c r="U22" t="n">
+        <v>211.730033990944</v>
       </c>
     </row>
     <row r="23">
@@ -2081,15 +2133,17 @@
       <c r="Q23" t="n">
         <v>0.0004286968068274045</v>
       </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>[0.00605723]</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>[240.40125743]</t>
-        </is>
+      <c r="R23" t="n">
+        <v>0.006057229858952722</v>
+      </c>
+      <c r="S23" t="n">
+        <v>240.4012574278262</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.0606128507806293</v>
+      </c>
+      <c r="U23" t="n">
+        <v>253.567507704706</v>
       </c>
     </row>
     <row r="24">
@@ -2152,15 +2206,17 @@
       <c r="Q24" t="n">
         <v>-9.209623205211912e-05</v>
       </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>[0.00585036]</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>[228.53323184]</t>
-        </is>
+      <c r="R24" t="n">
+        <v>0.005850360467485641</v>
+      </c>
+      <c r="S24" t="n">
+        <v>228.5332318441081</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.05555043014252268</v>
+      </c>
+      <c r="U24" t="n">
+        <v>248.409143478597</v>
       </c>
     </row>
     <row r="25">
@@ -2223,15 +2279,17 @@
       <c r="Q25" t="n">
         <v>-7.758201511646372e-05</v>
       </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>[0.00586016]</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>[236.12430816]</t>
-        </is>
+      <c r="R25" t="n">
+        <v>0.005860164602788233</v>
+      </c>
+      <c r="S25" t="n">
+        <v>236.1243081588227</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.05623690138902044</v>
+      </c>
+      <c r="U25" t="n">
+        <v>252.242629039729</v>
       </c>
     </row>
     <row r="26">
@@ -2294,15 +2352,17 @@
       <c r="Q26" t="n">
         <v>0.0002957619767601969</v>
       </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>[0.00618052]</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>[236.04290754]</t>
-        </is>
+      <c r="R26" t="n">
+        <v>0.006180515966385297</v>
+      </c>
+      <c r="S26" t="n">
+        <v>236.0429075417685</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.055440394783417</v>
+      </c>
+      <c r="U26" t="n">
+        <v>252.400500707896</v>
       </c>
     </row>
     <row r="27">
@@ -2365,15 +2425,17 @@
       <c r="Q27" t="n">
         <v>-0.0002421665394191476</v>
       </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>[0.00625276]</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>[249.03406727]</t>
-        </is>
+      <c r="R27" t="n">
+        <v>0.00625276335431681</v>
+      </c>
+      <c r="S27" t="n">
+        <v>249.0340672740449</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.08676426820902705</v>
+      </c>
+      <c r="U27" t="n">
+        <v>271.291495142471</v>
       </c>
     </row>
     <row r="28">
@@ -2436,15 +2498,17 @@
       <c r="Q28" t="n">
         <v>0.0004348944450230073</v>
       </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>[0.00608051]</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>[249.6013985]</t>
-        </is>
+      <c r="R28" t="n">
+        <v>0.006080505288134346</v>
+      </c>
+      <c r="S28" t="n">
+        <v>249.6013985008044</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.08765219920682091</v>
+      </c>
+      <c r="U28" t="n">
+        <v>271.450873256742</v>
       </c>
     </row>
     <row r="29">
@@ -2507,15 +2571,17 @@
       <c r="Q29" t="n">
         <v>-1.811243338828211e-05</v>
       </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>[0.00604259]</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>[247.44590736]</t>
-        </is>
+      <c r="R29" t="n">
+        <v>0.006042591421620828</v>
+      </c>
+      <c r="S29" t="n">
+        <v>247.4459073619275</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.09052019616698781</v>
+      </c>
+      <c r="U29" t="n">
+        <v>270.205556838554</v>
       </c>
     </row>
     <row r="30">
@@ -2578,15 +2644,17 @@
       <c r="Q30" t="n">
         <v>9.650639171126857e-05</v>
       </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>[0.00562653]</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>[243.56803442]</t>
-        </is>
+      <c r="R30" t="n">
+        <v>0.00562653037186802</v>
+      </c>
+      <c r="S30" t="n">
+        <v>243.5680344239455</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.06791943798146087</v>
+      </c>
+      <c r="U30" t="n">
+        <v>263.604579125519</v>
       </c>
     </row>
     <row r="31">
@@ -2649,15 +2717,17 @@
       <c r="Q31" t="n">
         <v>0.001050742857985741</v>
       </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>[0.0070141]</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>[247.25043481]</t>
-        </is>
+      <c r="R31" t="n">
+        <v>0.007014095061474104</v>
+      </c>
+      <c r="S31" t="n">
+        <v>247.2504348145901</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.06481664083431145</v>
+      </c>
+      <c r="U31" t="n">
+        <v>264.757089651222</v>
       </c>
     </row>
     <row r="32">
@@ -2720,15 +2790,17 @@
       <c r="Q32" t="n">
         <v>-4.507463801850802e-05</v>
       </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>[0.00493244]</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>[249.55500899]</t>
-        </is>
+      <c r="R32" t="n">
+        <v>0.00493244151691097</v>
+      </c>
+      <c r="S32" t="n">
+        <v>249.5550089922701</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.0724968705208921</v>
+      </c>
+      <c r="U32" t="n">
+        <v>271.657851543928</v>
       </c>
     </row>
     <row r="33">
@@ -2791,15 +2863,17 @@
       <c r="Q33" t="n">
         <v>0.0006475197704802183</v>
       </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>[0.00639713]</t>
-        </is>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>[237.75820578]</t>
-        </is>
+      <c r="R33" t="n">
+        <v>0.006397126507026385</v>
+      </c>
+      <c r="S33" t="n">
+        <v>237.7582057803729</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.06327855230482841</v>
+      </c>
+      <c r="U33" t="n">
+        <v>253.493165069991</v>
       </c>
     </row>
     <row r="34">
@@ -2862,15 +2936,17 @@
       <c r="Q34" t="n">
         <v>1.660443807201283e-06</v>
       </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>[0.00507792]</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>[234.17396009]</t>
-        </is>
+      <c r="R34" t="n">
+        <v>0.0050779215058355</v>
+      </c>
+      <c r="S34" t="n">
+        <v>234.1739600944735</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.0581172248841626</v>
+      </c>
+      <c r="U34" t="n">
+        <v>250.46657626376</v>
       </c>
     </row>
     <row r="35">
@@ -2933,15 +3009,17 @@
       <c r="Q35" t="n">
         <v>4.135819297285646e-05</v>
       </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>[0.00557583]</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>[235.16789173]</t>
-        </is>
+      <c r="R35" t="n">
+        <v>0.00557582768434924</v>
+      </c>
+      <c r="S35" t="n">
+        <v>235.1678917258114</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.06177096046406755</v>
+      </c>
+      <c r="U35" t="n">
+        <v>251.402613069041</v>
       </c>
     </row>
     <row r="36">
@@ -3004,15 +3082,17 @@
       <c r="Q36" t="n">
         <v>0.001131404196779302</v>
       </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>[0.00694048]</t>
-        </is>
-      </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>[274.25136363]</t>
-        </is>
+      <c r="R36" t="n">
+        <v>0.006940478529454215</v>
+      </c>
+      <c r="S36" t="n">
+        <v>274.2513636288905</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.1039466137058933</v>
+      </c>
+      <c r="U36" t="n">
+        <v>293.397949120819</v>
       </c>
     </row>
     <row r="37">
@@ -3075,15 +3155,17 @@
       <c r="Q37" t="n">
         <v>0.0009057003101174462</v>
       </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>[0.00785175]</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>[262.3832283]</t>
-        </is>
+      <c r="R37" t="n">
+        <v>0.007851750173183051</v>
+      </c>
+      <c r="S37" t="n">
+        <v>262.3832283021977</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.06776913790716595</v>
+      </c>
+      <c r="U37" t="n">
+        <v>275.464486634296</v>
       </c>
     </row>
     <row r="38">
@@ -3146,15 +3228,17 @@
       <c r="Q38" t="n">
         <v>0.0008630670852242486</v>
       </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>[0.00699255]</t>
-        </is>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>[272.27523845]</t>
-        </is>
+      <c r="R38" t="n">
+        <v>0.006992552239309712</v>
+      </c>
+      <c r="S38" t="n">
+        <v>272.2752384546816</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0.07524613817692086</v>
+      </c>
+      <c r="U38" t="n">
+        <v>287.549644301715</v>
       </c>
     </row>
     <row r="39">
@@ -3217,15 +3301,17 @@
       <c r="Q39" t="n">
         <v>0.0008016758350805884</v>
       </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>[0.00707856]</t>
-        </is>
-      </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>[253.21952832]</t>
-        </is>
+      <c r="R39" t="n">
+        <v>0.007078556099443474</v>
+      </c>
+      <c r="S39" t="n">
+        <v>253.2195283238483</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.0791963072283015</v>
+      </c>
+      <c r="U39" t="n">
+        <v>265.015192851842</v>
       </c>
     </row>
     <row r="40">
@@ -3288,15 +3374,17 @@
       <c r="Q40" t="n">
         <v>1.049680261430187e-05</v>
       </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>[0.00570956]</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>[213.2409893]</t>
-        </is>
+      <c r="R40" t="n">
+        <v>0.005709563271638576</v>
+      </c>
+      <c r="S40" t="n">
+        <v>213.2409893003532</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0.0304411103719273</v>
+      </c>
+      <c r="U40" t="n">
+        <v>216.514566785978</v>
       </c>
     </row>
     <row r="41">
@@ -3359,15 +3447,17 @@
       <c r="Q41" t="n">
         <v>0.0001231640292093314</v>
       </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>[0.00610135]</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>[213.67688741]</t>
-        </is>
+      <c r="R41" t="n">
+        <v>0.006101346774042363</v>
+      </c>
+      <c r="S41" t="n">
+        <v>213.6768874072478</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0.03402964946458783</v>
+      </c>
+      <c r="U41" t="n">
+        <v>217.172642097812</v>
       </c>
     </row>
     <row r="42">
@@ -3430,15 +3520,17 @@
       <c r="Q42" t="n">
         <v>0.0007330792019057392</v>
       </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>[0.00607948]</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>[229.77271333]</t>
-        </is>
+      <c r="R42" t="n">
+        <v>0.006079483160420184</v>
+      </c>
+      <c r="S42" t="n">
+        <v>229.7727133278009</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0.04339486322370684</v>
+      </c>
+      <c r="U42" t="n">
+        <v>240.849767014709</v>
       </c>
     </row>
     <row r="43">
@@ -3501,15 +3593,17 @@
       <c r="Q43" t="n">
         <v>0.000875812239462738</v>
       </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>[0.00689806]</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>[231.37142148]</t>
-        </is>
+      <c r="R43" t="n">
+        <v>0.006898064852333649</v>
+      </c>
+      <c r="S43" t="n">
+        <v>231.3714214804136</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0.04904562034392084</v>
+      </c>
+      <c r="U43" t="n">
+        <v>240.674565948934</v>
       </c>
     </row>
     <row r="44">
@@ -3572,15 +3666,17 @@
       <c r="Q44" t="n">
         <v>0.0007321093497570839</v>
       </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>[0.00680595]</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>[229.41907001]</t>
-        </is>
+      <c r="R44" t="n">
+        <v>0.006805946797575814</v>
+      </c>
+      <c r="S44" t="n">
+        <v>229.4190700061421</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0.04047712239809449</v>
+      </c>
+      <c r="U44" t="n">
+        <v>237.543726708187</v>
       </c>
     </row>
     <row r="45">
@@ -3643,15 +3739,17 @@
       <c r="Q45" t="n">
         <v>0.001030591323611097</v>
       </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>[0.00729047]</t>
-        </is>
-      </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>[230.18281857]</t>
-        </is>
+      <c r="R45" t="n">
+        <v>0.007290473730071174</v>
+      </c>
+      <c r="S45" t="n">
+        <v>230.1828185656784</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0.0391739557928488</v>
+      </c>
+      <c r="U45" t="n">
+        <v>236.712298530189</v>
       </c>
     </row>
     <row r="46">
@@ -3714,15 +3812,17 @@
       <c r="Q46" t="n">
         <v>0.0004840251368253188</v>
       </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>[0.00607457]</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>[197.36300395]</t>
-        </is>
+      <c r="R46" t="n">
+        <v>0.006074571574026012</v>
+      </c>
+      <c r="S46" t="n">
+        <v>197.3630039470384</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0.03642337811914912</v>
+      </c>
+      <c r="U46" t="n">
+        <v>202.543443662674</v>
       </c>
     </row>
     <row r="47">
@@ -3785,15 +3885,17 @@
       <c r="Q47" t="n">
         <v>0.0005983305746827686</v>
       </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>[0.00608636]</t>
-        </is>
-      </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>[216.34693032]</t>
-        </is>
+      <c r="R47" t="n">
+        <v>0.006086361557137697</v>
+      </c>
+      <c r="S47" t="n">
+        <v>216.3469303180482</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0.03656730470412467</v>
+      </c>
+      <c r="U47" t="n">
+        <v>221.255129744395</v>
       </c>
     </row>
     <row r="48">
@@ -3856,15 +3958,17 @@
       <c r="Q48" t="n">
         <v>8.460631615250054e-05</v>
       </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>[0.00675115]</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>[247.59971195]</t>
-        </is>
+      <c r="R48" t="n">
+        <v>0.006751154581737274</v>
+      </c>
+      <c r="S48" t="n">
+        <v>247.599711952659</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0.0512976328902893</v>
+      </c>
+      <c r="U48" t="n">
+        <v>255.363733076386</v>
       </c>
     </row>
     <row r="49">
@@ -3927,15 +4031,17 @@
       <c r="Q49" t="n">
         <v>0.0008567276039679844</v>
       </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>[0.00726536]</t>
-        </is>
-      </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>[240.59583819]</t>
-        </is>
+      <c r="R49" t="n">
+        <v>0.007265361413355857</v>
+      </c>
+      <c r="S49" t="n">
+        <v>240.5958381886858</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0.006497023365769584</v>
+      </c>
+      <c r="U49" t="n">
+        <v>241.10099190058</v>
       </c>
     </row>
     <row r="50">
@@ -3998,15 +4104,17 @@
       <c r="Q50" t="n">
         <v>0.0002699520485847642</v>
       </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>[0.00682053]</t>
-        </is>
-      </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>[254.63062289]</t>
-        </is>
+      <c r="R50" t="n">
+        <v>0.006820531552530755</v>
+      </c>
+      <c r="S50" t="n">
+        <v>254.6306228924357</v>
+      </c>
+      <c r="T50" t="n">
+        <v>0.04118873217523027</v>
+      </c>
+      <c r="U50" t="n">
+        <v>259.309388683401</v>
       </c>
     </row>
     <row r="51">
@@ -4069,15 +4177,17 @@
       <c r="Q51" t="n">
         <v>0.001260259507802939</v>
       </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>[0.00796062]</t>
-        </is>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>[241.39220896]</t>
-        </is>
+      <c r="R51" t="n">
+        <v>0.007960622345647822</v>
+      </c>
+      <c r="S51" t="n">
+        <v>241.3922089625397</v>
+      </c>
+      <c r="T51" t="n">
+        <v>0.008242619041144239</v>
+      </c>
+      <c r="U51" t="n">
+        <v>241.484548491853</v>
       </c>
     </row>
     <row r="52">
@@ -4144,15 +4254,17 @@
       <c r="Q52" t="n">
         <v>0.00132275994714398</v>
       </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>[0.00634629]</t>
-        </is>
-      </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>[191.29395231]</t>
-        </is>
+      <c r="R52" t="n">
+        <v>0.006346293711635107</v>
+      </c>
+      <c r="S52" t="n">
+        <v>191.2939523065533</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0.00600200521670768</v>
+      </c>
+      <c r="U52" t="n">
+        <v>191.370191541496</v>
       </c>
     </row>
     <row r="53">
@@ -4215,15 +4327,17 @@
       <c r="Q53" t="n">
         <v>0.0005956601279578689</v>
       </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>[0.00545578]</t>
-        </is>
-      </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>[186.76539531]</t>
-        </is>
+      <c r="R53" t="n">
+        <v>0.005455781228274737</v>
+      </c>
+      <c r="S53" t="n">
+        <v>186.7653953109622</v>
+      </c>
+      <c r="T53" t="n">
+        <v>0.006136977316196669</v>
+      </c>
+      <c r="U53" t="n">
+        <v>187.063802254395</v>
       </c>
     </row>
     <row r="54">
@@ -4286,15 +4400,17 @@
       <c r="Q54" t="n">
         <v>0.0002364311953404587</v>
       </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>[0.00465399]</t>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>[153.96170388]</t>
-        </is>
+      <c r="R54" t="n">
+        <v>0.004653991672311814</v>
+      </c>
+      <c r="S54" t="n">
+        <v>153.961703875818</v>
+      </c>
+      <c r="T54" t="n">
+        <v>0.006367422273143558</v>
+      </c>
+      <c r="U54" t="n">
+        <v>155.542029266887</v>
       </c>
     </row>
     <row r="55">
@@ -4357,15 +4473,17 @@
       <c r="Q55" t="n">
         <v>6.444663434220649e-05</v>
       </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>[0.0054088]</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>[186.37201145]</t>
-        </is>
+      <c r="R55" t="n">
+        <v>0.005408804394300856</v>
+      </c>
+      <c r="S55" t="n">
+        <v>186.3720114492982</v>
+      </c>
+      <c r="T55" t="n">
+        <v>0.005961127594607606</v>
+      </c>
+      <c r="U55" t="n">
+        <v>186.424224049047</v>
       </c>
     </row>
     <row r="56">
@@ -4428,15 +4546,17 @@
       <c r="Q56" t="n">
         <v>0.0005357913646937737</v>
       </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>[0.00574067]</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>[187.39180035]</t>
-        </is>
+      <c r="R56" t="n">
+        <v>0.005740667863448074</v>
+      </c>
+      <c r="S56" t="n">
+        <v>187.3918003496629</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0.006069660719238274</v>
+      </c>
+      <c r="U56" t="n">
+        <v>187.450289031598</v>
       </c>
     </row>
     <row r="57">
@@ -4499,15 +4619,17 @@
       <c r="Q57" t="n">
         <v>0.0001747938059600222</v>
       </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>[0.00529155]</t>
-        </is>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>[191.95047384]</t>
-        </is>
+      <c r="R57" t="n">
+        <v>0.005291547287762345</v>
+      </c>
+      <c r="S57" t="n">
+        <v>191.9504738433116</v>
+      </c>
+      <c r="T57" t="n">
+        <v>0.004750452684039422</v>
+      </c>
+      <c r="U57" t="n">
+        <v>192.145019792861</v>
       </c>
     </row>
     <row r="58">
@@ -4570,15 +4692,17 @@
       <c r="Q58" t="n">
         <v>0.001127086786231615</v>
       </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>[0.00658279]</t>
-        </is>
-      </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>[202.89022806]</t>
-        </is>
+      <c r="R58" t="n">
+        <v>0.006582794824301516</v>
+      </c>
+      <c r="S58" t="n">
+        <v>202.8902280586657</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0.01307175397844072</v>
+      </c>
+      <c r="U58" t="n">
+        <v>204.264655235437</v>
       </c>
     </row>
     <row r="59">
@@ -4645,15 +4769,17 @@
       <c r="Q59" t="n">
         <v>0.001142736282227179</v>
       </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>[0.00663262]</t>
-        </is>
-      </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>[200.59782047]</t>
-        </is>
+      <c r="R59" t="n">
+        <v>0.006632619059514852</v>
+      </c>
+      <c r="S59" t="n">
+        <v>200.5978204731842</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0.01207331893905818</v>
+      </c>
+      <c r="U59" t="n">
+        <v>202.162945055175</v>
       </c>
     </row>
     <row r="60">
@@ -4716,15 +4842,17 @@
       <c r="Q60" t="n">
         <v>0.0002063811979691773</v>
       </c>
-      <c r="R60" t="inlineStr">
-        <is>
-          <t>[0.00580383]</t>
-        </is>
-      </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>[198.98072405]</t>
-        </is>
+      <c r="R60" t="n">
+        <v>0.005803834383658227</v>
+      </c>
+      <c r="S60" t="n">
+        <v>198.9807240515658</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0.01485101692437998</v>
+      </c>
+      <c r="U60" t="n">
+        <v>202.03588317029</v>
       </c>
     </row>
     <row r="61">
@@ -4787,15 +4915,17 @@
       <c r="Q61" t="n">
         <v>0.0003618505727106058</v>
       </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>[0.00573765]</t>
-        </is>
-      </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>[205.94279353]</t>
-        </is>
+      <c r="R61" t="n">
+        <v>0.005737648247877516</v>
+      </c>
+      <c r="S61" t="n">
+        <v>205.9427935256723</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0.01167385278745861</v>
+      </c>
+      <c r="U61" t="n">
+        <v>209.137978876701</v>
       </c>
     </row>
     <row r="62">
@@ -4858,15 +4988,17 @@
       <c r="Q62" t="n">
         <v>0.0009129031790100989</v>
       </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>[0.00663551]</t>
-        </is>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>[188.02936756]</t>
-        </is>
+      <c r="R62" t="n">
+        <v>0.006635512021630569</v>
+      </c>
+      <c r="S62" t="n">
+        <v>188.0293675592692</v>
+      </c>
+      <c r="T62" t="n">
+        <v>0.0125276350596358</v>
+      </c>
+      <c r="U62" t="n">
+        <v>189.531829382623</v>
       </c>
     </row>
     <row r="63">
@@ -4929,15 +5061,17 @@
       <c r="Q63" t="n">
         <v>-1.666305095732092e-05</v>
       </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>[0.00578348]</t>
-        </is>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>[193.90783315]</t>
-        </is>
+      <c r="R63" t="n">
+        <v>0.005783477422261261</v>
+      </c>
+      <c r="S63" t="n">
+        <v>193.9078331451065</v>
+      </c>
+      <c r="T63" t="n">
+        <v>0.01022459388214218</v>
+      </c>
+      <c r="U63" t="n">
+        <v>195.427940959688</v>
       </c>
     </row>
     <row r="64">
@@ -5000,15 +5134,17 @@
       <c r="Q64" t="n">
         <v>-5.101728079533185e-05</v>
       </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>[0.00566904]</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>[182.07793808]</t>
-        </is>
+      <c r="R64" t="n">
+        <v>0.005669044888643195</v>
+      </c>
+      <c r="S64" t="n">
+        <v>182.0779380765711</v>
+      </c>
+      <c r="T64" t="n">
+        <v>0.009011824012097068</v>
+      </c>
+      <c r="U64" t="n">
+        <v>183.619171087842</v>
       </c>
     </row>
     <row r="65">
@@ -5071,15 +5207,17 @@
       <c r="Q65" t="n">
         <v>1.674164147798338e-06</v>
       </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>[0.00579331]</t>
-        </is>
-      </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>[186.23587121]</t>
-        </is>
+      <c r="R65" t="n">
+        <v>0.005793306344620133</v>
+      </c>
+      <c r="S65" t="n">
+        <v>186.2358712124743</v>
+      </c>
+      <c r="T65" t="n">
+        <v>0.008849549396020399</v>
+      </c>
+      <c r="U65" t="n">
+        <v>187.535587283919</v>
       </c>
     </row>
     <row r="66">
@@ -5146,15 +5284,17 @@
       <c r="Q66" t="n">
         <v>9.552114163655697e-05</v>
       </c>
-      <c r="R66" t="inlineStr">
-        <is>
-          <t>[0.00581521]</t>
-        </is>
-      </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>[184.28113182]</t>
-        </is>
+      <c r="R66" t="n">
+        <v>0.005815206931334676</v>
+      </c>
+      <c r="S66" t="n">
+        <v>184.2811318223662</v>
+      </c>
+      <c r="T66" t="n">
+        <v>0.008711586469099059</v>
+      </c>
+      <c r="U66" t="n">
+        <v>185.133067248502</v>
       </c>
     </row>
     <row r="67">
@@ -5217,15 +5357,17 @@
       <c r="Q67" t="n">
         <v>0.001640142602827623</v>
       </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>[0.00681378]</t>
-        </is>
-      </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>[203.79857259]</t>
-        </is>
+      <c r="R67" t="n">
+        <v>0.006813778342915136</v>
+      </c>
+      <c r="S67" t="n">
+        <v>203.7985725903647</v>
+      </c>
+      <c r="T67" t="n">
+        <v>0.01550590806628042</v>
+      </c>
+      <c r="U67" t="n">
+        <v>210.466086428666</v>
       </c>
     </row>
     <row r="68">
@@ -5292,15 +5434,17 @@
       <c r="Q68" t="n">
         <v>0.0008713315624624507</v>
       </c>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>[0.00699032]</t>
-        </is>
-      </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>[204.65696578]</t>
-        </is>
+      <c r="R68" t="n">
+        <v>0.006990320595614026</v>
+      </c>
+      <c r="S68" t="n">
+        <v>204.6569657797569</v>
+      </c>
+      <c r="T68" t="n">
+        <v>0.007071893132006251</v>
+      </c>
+      <c r="U68" t="n">
+        <v>204.657485228647</v>
       </c>
     </row>
     <row r="69">
@@ -5363,15 +5507,17 @@
       <c r="Q69" t="n">
         <v>0.0008277733694668681</v>
       </c>
-      <c r="R69" t="inlineStr">
-        <is>
-          <t>[0.0071111]</t>
-        </is>
-      </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>[222.92474578]</t>
-        </is>
+      <c r="R69" t="n">
+        <v>0.0071110979263226</v>
+      </c>
+      <c r="S69" t="n">
+        <v>222.924745775949</v>
+      </c>
+      <c r="T69" t="n">
+        <v>0.01145801644128087</v>
+      </c>
+      <c r="U69" t="n">
+        <v>224.872007907994</v>
       </c>
     </row>
     <row r="70">
@@ -5434,15 +5580,17 @@
       <c r="Q70" t="n">
         <v>0.0008636320765332151</v>
       </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>[0.0073493]</t>
-        </is>
-      </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>[211.28392598]</t>
-        </is>
+      <c r="R70" t="n">
+        <v>0.007349302068520335</v>
+      </c>
+      <c r="S70" t="n">
+        <v>211.2839259816319</v>
+      </c>
+      <c r="T70" t="n">
+        <v>0.007606621553771215</v>
+      </c>
+      <c r="U70" t="n">
+        <v>211.331962991235</v>
       </c>
     </row>
     <row r="71">
@@ -5505,15 +5653,17 @@
       <c r="Q71" t="n">
         <v>0.0003898922701446438</v>
       </c>
-      <c r="R71" t="inlineStr">
-        <is>
-          <t>[0.00546613]</t>
-        </is>
-      </c>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>[129.6889121]</t>
-        </is>
+      <c r="R71" t="n">
+        <v>0.00546613076882481</v>
+      </c>
+      <c r="S71" t="n">
+        <v>129.6889121000877</v>
+      </c>
+      <c r="T71" t="n">
+        <v>0.007799409260379744</v>
+      </c>
+      <c r="U71" t="n">
+        <v>134.69393694681</v>
       </c>
     </row>
     <row r="72">
@@ -5565,7 +5715,7 @@
         <v>47.3625404782615</v>
       </c>
       <c r="N72" t="n">
-        <v>42175.08103243844</v>
+        <v>42175.08103243845</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5574,17 +5724,19 @@
       </c>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="n">
-        <v>0.0006093202581949112</v>
-      </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>[0.00514178]</t>
-        </is>
-      </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>[132.50463468]</t>
-        </is>
+        <v>0.0006093202581949108</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0.005141775461653572</v>
+      </c>
+      <c r="S72" t="n">
+        <v>132.5046346809661</v>
+      </c>
+      <c r="T72" t="n">
+        <v>0.00634969439522871</v>
+      </c>
+      <c r="U72" t="n">
+        <v>133.309917226322</v>
       </c>
     </row>
     <row r="73">
@@ -5647,15 +5799,17 @@
       <c r="Q73" t="n">
         <v>0.0008211559912235707</v>
       </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>[0.00605676]</t>
-        </is>
-      </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>[141.60878781]</t>
-        </is>
+      <c r="R73" t="n">
+        <v>0.006056757265215473</v>
+      </c>
+      <c r="S73" t="n">
+        <v>141.6087878107656</v>
+      </c>
+      <c r="T73" t="n">
+        <v>0.006845716453860471</v>
+      </c>
+      <c r="U73" t="n">
+        <v>141.780138833582</v>
       </c>
     </row>
     <row r="74">
@@ -5718,15 +5872,17 @@
       <c r="Q74" t="n">
         <v>0.0007788589957005581</v>
       </c>
-      <c r="R74" t="inlineStr">
-        <is>
-          <t>[0.00557443]</t>
-        </is>
-      </c>
-      <c r="S74" t="inlineStr">
-        <is>
-          <t>[136.21916497]</t>
-        </is>
+      <c r="R74" t="n">
+        <v>0.00557442890688067</v>
+      </c>
+      <c r="S74" t="n">
+        <v>136.2191649697395</v>
+      </c>
+      <c r="T74" t="n">
+        <v>0.007189168888577158</v>
+      </c>
+      <c r="U74" t="n">
+        <v>136.660030904845</v>
       </c>
     </row>
     <row r="75">
@@ -5789,15 +5945,17 @@
       <c r="Q75" t="n">
         <v>0.0005373300618622199</v>
       </c>
-      <c r="R75" t="inlineStr">
-        <is>
-          <t>[0.00462111]</t>
-        </is>
-      </c>
-      <c r="S75" t="inlineStr">
-        <is>
-          <t>[141.22362941]</t>
-        </is>
+      <c r="R75" t="n">
+        <v>0.004621107738568818</v>
+      </c>
+      <c r="S75" t="n">
+        <v>141.2236294072566</v>
+      </c>
+      <c r="T75" t="n">
+        <v>0.006629490100595221</v>
+      </c>
+      <c r="U75" t="n">
+        <v>142.958823169674</v>
       </c>
     </row>
     <row r="76">
@@ -5860,15 +6018,17 @@
       <c r="Q76" t="n">
         <v>0.001074375897386028</v>
       </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>[0.00564098]</t>
-        </is>
-      </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>[136.3471848]</t>
-        </is>
+      <c r="R76" t="n">
+        <v>0.00564098133698432</v>
+      </c>
+      <c r="S76" t="n">
+        <v>136.3471848029357</v>
+      </c>
+      <c r="T76" t="n">
+        <v>0.007175549824161928</v>
+      </c>
+      <c r="U76" t="n">
+        <v>137.179821141542</v>
       </c>
     </row>
     <row r="77">
@@ -5931,15 +6091,17 @@
       <c r="Q77" t="n">
         <v>0.0006566808991932407</v>
       </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>[0.00533035]</t>
-        </is>
-      </c>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>[130.03415098]</t>
-        </is>
+      <c r="R77" t="n">
+        <v>0.005330352662962963</v>
+      </c>
+      <c r="S77" t="n">
+        <v>130.0341509768202</v>
+      </c>
+      <c r="T77" t="n">
+        <v>0.006219257711500141</v>
+      </c>
+      <c r="U77" t="n">
+        <v>130.664513249855</v>
       </c>
     </row>
     <row r="78">
@@ -6002,15 +6164,17 @@
       <c r="Q78" t="n">
         <v>0.001021084008256706</v>
       </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>[0.0058033]</t>
-        </is>
-      </c>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>[143.95125506]</t>
-        </is>
+      <c r="R78" t="n">
+        <v>0.005803303453432615</v>
+      </c>
+      <c r="S78" t="n">
+        <v>143.951255063073</v>
+      </c>
+      <c r="T78" t="n">
+        <v>0.006927624270495906</v>
+      </c>
+      <c r="U78" t="n">
+        <v>144.414772365256</v>
       </c>
     </row>
     <row r="79">
@@ -6073,15 +6237,17 @@
       <c r="Q79" t="n">
         <v>0.0001476417332973139</v>
       </c>
-      <c r="R79" t="inlineStr">
-        <is>
-          <t>[0.00536874]</t>
-        </is>
-      </c>
-      <c r="S79" t="inlineStr">
-        <is>
-          <t>[145.60052924]</t>
-        </is>
+      <c r="R79" t="n">
+        <v>0.005368738589116732</v>
+      </c>
+      <c r="S79" t="n">
+        <v>145.6005292377227</v>
+      </c>
+      <c r="T79" t="n">
+        <v>0.007845307566702913</v>
+      </c>
+      <c r="U79" t="n">
+        <v>148.580738463673</v>
       </c>
     </row>
     <row r="80">
@@ -6144,15 +6310,17 @@
       <c r="Q80" t="n">
         <v>0.0006196032013576478</v>
       </c>
-      <c r="R80" t="inlineStr">
-        <is>
-          <t>[0.00592656]</t>
-        </is>
-      </c>
-      <c r="S80" t="inlineStr">
-        <is>
-          <t>[139.29562962]</t>
-        </is>
+      <c r="R80" t="n">
+        <v>0.005926556948214083</v>
+      </c>
+      <c r="S80" t="n">
+        <v>139.2956296195097</v>
+      </c>
+      <c r="T80" t="n">
+        <v>0.006640548661777547</v>
+      </c>
+      <c r="U80" t="n">
+        <v>139.448240759938</v>
       </c>
     </row>
     <row r="81">
@@ -6215,15 +6383,17 @@
       <c r="Q81" t="n">
         <v>0.0002125575271850833</v>
       </c>
-      <c r="R81" t="inlineStr">
-        <is>
-          <t>[0.00580823]</t>
-        </is>
-      </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>[166.60858725]</t>
-        </is>
+      <c r="R81" t="n">
+        <v>0.005808227632039806</v>
+      </c>
+      <c r="S81" t="n">
+        <v>166.6085872526358</v>
+      </c>
+      <c r="T81" t="n">
+        <v>0.006633700577796983</v>
+      </c>
+      <c r="U81" t="n">
+        <v>166.955090490534</v>
       </c>
     </row>
     <row r="82">
@@ -6286,15 +6456,17 @@
       <c r="Q82" t="n">
         <v>0.000333785642721991</v>
       </c>
-      <c r="R82" t="inlineStr">
-        <is>
-          <t>[0.00507381]</t>
-        </is>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>[144.6287459]</t>
-        </is>
+      <c r="R82" t="n">
+        <v>0.005073806151259936</v>
+      </c>
+      <c r="S82" t="n">
+        <v>144.6287458969511</v>
+      </c>
+      <c r="T82" t="n">
+        <v>0.006315050455573591</v>
+      </c>
+      <c r="U82" t="n">
+        <v>145.695282847335</v>
       </c>
     </row>
     <row r="83">
@@ -6357,15 +6529,17 @@
       <c r="Q83" t="n">
         <v>0.0009347059551158865</v>
       </c>
-      <c r="R83" t="inlineStr">
-        <is>
-          <t>[0.0041256]</t>
-        </is>
-      </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>[69.54697523]</t>
-        </is>
+      <c r="R83" t="n">
+        <v>0.004125603225819556</v>
+      </c>
+      <c r="S83" t="n">
+        <v>69.54697523046757</v>
+      </c>
+      <c r="T83" t="n">
+        <v>0.01062249189701809</v>
+      </c>
+      <c r="U83" t="n">
+        <v>70.754951381214</v>
       </c>
     </row>
     <row r="84">
@@ -6428,15 +6602,17 @@
       <c r="Q84" t="n">
         <v>-0.0001436401650030661</v>
       </c>
-      <c r="R84" t="inlineStr">
-        <is>
-          <t>[0.0035729]</t>
-        </is>
-      </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>[78.98547761]</t>
-        </is>
+      <c r="R84" t="n">
+        <v>0.003572896668335576</v>
+      </c>
+      <c r="S84" t="n">
+        <v>78.98547761406947</v>
+      </c>
+      <c r="T84" t="n">
+        <v>0.007440856435661033</v>
+      </c>
+      <c r="U84" t="n">
+        <v>80.145734222926</v>
       </c>
     </row>
     <row r="85">
@@ -6499,15 +6675,17 @@
       <c r="Q85" t="n">
         <v>0.0001791885963953713</v>
       </c>
-      <c r="R85" t="inlineStr">
-        <is>
-          <t>[0.00401321]</t>
-        </is>
-      </c>
-      <c r="S85" t="inlineStr">
-        <is>
-          <t>[64.67745758]</t>
-        </is>
+      <c r="R85" t="n">
+        <v>0.004013207649416292</v>
+      </c>
+      <c r="S85" t="n">
+        <v>64.67745757601358</v>
+      </c>
+      <c r="T85" t="n">
+        <v>0.005221002964485771</v>
+      </c>
+      <c r="U85" t="n">
+        <v>64.900513332527</v>
       </c>
     </row>
     <row r="86">
@@ -6553,13 +6731,13 @@
         <v>57.0351509504363</v>
       </c>
       <c r="L86" t="n">
-        <v>0.0006235740665684951</v>
+        <v>0.0006235740665684949</v>
       </c>
       <c r="M86" t="n">
         <v>33.316765619273</v>
       </c>
       <c r="N86" t="n">
-        <v>53428.72227290324</v>
+        <v>53428.72227290325</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6568,17 +6746,19 @@
       </c>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="n">
-        <v>9.602688302589506e-05</v>
-      </c>
-      <c r="R86" t="inlineStr">
-        <is>
-          <t>[0.00356227]</t>
-        </is>
-      </c>
-      <c r="S86" t="inlineStr">
-        <is>
-          <t>[83.46997454]</t>
-        </is>
+        <v>9.602688302589484e-05</v>
+      </c>
+      <c r="R86" t="n">
+        <v>0.00356226783994753</v>
+      </c>
+      <c r="S86" t="n">
+        <v>83.46997453644505</v>
+      </c>
+      <c r="T86" t="n">
+        <v>0.005442698321062894</v>
+      </c>
+      <c r="U86" t="n">
+        <v>83.72798804076319</v>
       </c>
     </row>
     <row r="87">
@@ -6641,15 +6821,17 @@
       <c r="Q87" t="n">
         <v>-0.0009169705344778045</v>
       </c>
-      <c r="R87" t="inlineStr">
-        <is>
-          <t>[0.00384293]</t>
-        </is>
-      </c>
-      <c r="S87" t="inlineStr">
-        <is>
-          <t>[79.88715192]</t>
-        </is>
+      <c r="R87" t="n">
+        <v>0.003842934907925612</v>
+      </c>
+      <c r="S87" t="n">
+        <v>79.88715192467411</v>
+      </c>
+      <c r="T87" t="n">
+        <v>0.008634918362270396</v>
+      </c>
+      <c r="U87" t="n">
+        <v>84.5334661269134</v>
       </c>
     </row>
     <row r="88">
@@ -6712,15 +6894,17 @@
       <c r="Q88" t="n">
         <v>0.0001588269294999108</v>
       </c>
-      <c r="R88" t="inlineStr">
-        <is>
-          <t>[0.00331263]</t>
-        </is>
-      </c>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>[80.71874585]</t>
-        </is>
+      <c r="R88" t="n">
+        <v>0.003312626263537214</v>
+      </c>
+      <c r="S88" t="n">
+        <v>80.71874585467015</v>
+      </c>
+      <c r="T88" t="n">
+        <v>0.005567210069652111</v>
+      </c>
+      <c r="U88" t="n">
+        <v>81.0843557964908</v>
       </c>
     </row>
     <row r="89">
@@ -6783,15 +6967,17 @@
       <c r="Q89" t="n">
         <v>0.0003953219097204959</v>
       </c>
-      <c r="R89" t="inlineStr">
-        <is>
-          <t>[0.00411088]</t>
-        </is>
-      </c>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>[85.28803901]</t>
-        </is>
+      <c r="R89" t="n">
+        <v>0.00411088376482903</v>
+      </c>
+      <c r="S89" t="n">
+        <v>85.28803901052348</v>
+      </c>
+      <c r="T89" t="n">
+        <v>0.007758465815029795</v>
+      </c>
+      <c r="U89" t="n">
+        <v>86.0178561758589</v>
       </c>
     </row>
     <row r="90">
@@ -6854,15 +7040,17 @@
       <c r="Q90" t="n">
         <v>0.000458888064130165</v>
       </c>
-      <c r="R90" t="inlineStr">
-        <is>
-          <t>[0.00418117]</t>
-        </is>
-      </c>
-      <c r="S90" t="inlineStr">
-        <is>
-          <t>[91.40909649]</t>
-        </is>
+      <c r="R90" t="n">
+        <v>0.004181172884509807</v>
+      </c>
+      <c r="S90" t="n">
+        <v>91.40909649393312</v>
+      </c>
+      <c r="T90" t="n">
+        <v>0.006129862488138665</v>
+      </c>
+      <c r="U90" t="n">
+        <v>92.5678234692284</v>
       </c>
     </row>
     <row r="91">
@@ -6925,15 +7113,17 @@
       <c r="Q91" t="n">
         <v>-1.897273397861131e-05</v>
       </c>
-      <c r="R91" t="inlineStr">
-        <is>
-          <t>[0.00384502]</t>
-        </is>
-      </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>[100.32410037]</t>
-        </is>
+      <c r="R91" t="n">
+        <v>0.003845015090834731</v>
+      </c>
+      <c r="S91" t="n">
+        <v>100.3241003734969</v>
+      </c>
+      <c r="T91" t="n">
+        <v>0.005400590477398788</v>
+      </c>
+      <c r="U91" t="n">
+        <v>101.135274005206</v>
       </c>
     </row>
     <row r="92">
@@ -6996,15 +7186,17 @@
       <c r="Q92" t="n">
         <v>-0.0001868859276654517</v>
       </c>
-      <c r="R92" t="inlineStr">
-        <is>
-          <t>[0.00382425]</t>
-        </is>
-      </c>
-      <c r="S92" t="inlineStr">
-        <is>
-          <t>[79.79221366]</t>
-        </is>
+      <c r="R92" t="n">
+        <v>0.003824251563732763</v>
+      </c>
+      <c r="S92" t="n">
+        <v>79.79221366062833</v>
+      </c>
+      <c r="T92" t="n">
+        <v>0.008370099529723349</v>
+      </c>
+      <c r="U92" t="n">
+        <v>80.7594992735058</v>
       </c>
     </row>
     <row r="93">
@@ -7067,15 +7259,17 @@
       <c r="Q93" t="n">
         <v>0.001262320824785163</v>
       </c>
-      <c r="R93" t="inlineStr">
-        <is>
-          <t>[0.00485937]</t>
-        </is>
-      </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>[82.96977647]</t>
-        </is>
+      <c r="R93" t="n">
+        <v>0.004859365869035659</v>
+      </c>
+      <c r="S93" t="n">
+        <v>82.9697764667787</v>
+      </c>
+      <c r="T93" t="n">
+        <v>0.007047322469866863</v>
+      </c>
+      <c r="U93" t="n">
+        <v>84.22521596624161</v>
       </c>
     </row>
     <row r="94">
@@ -7138,15 +7332,17 @@
       <c r="Q94" t="n">
         <v>-0.0003254508736255729</v>
       </c>
-      <c r="R94" t="inlineStr">
-        <is>
-          <t>[0.00392154]</t>
-        </is>
-      </c>
-      <c r="S94" t="inlineStr">
-        <is>
-          <t>[87.14115823]</t>
-        </is>
+      <c r="R94" t="n">
+        <v>0.003921538998074458</v>
+      </c>
+      <c r="S94" t="n">
+        <v>87.14115823124914</v>
+      </c>
+      <c r="T94" t="n">
+        <v>0.007259205002188027</v>
+      </c>
+      <c r="U94" t="n">
+        <v>90.1074544338652</v>
       </c>
     </row>
     <row r="95">
@@ -7209,15 +7405,17 @@
       <c r="Q95" t="n">
         <v>-0.0002985639296833897</v>
       </c>
-      <c r="R95" t="inlineStr">
-        <is>
-          <t>[0.00376918]</t>
-        </is>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>[80.63825522]</t>
-        </is>
+      <c r="R95" t="n">
+        <v>0.003769177417556691</v>
+      </c>
+      <c r="S95" t="n">
+        <v>80.63825521521659</v>
+      </c>
+      <c r="T95" t="n">
+        <v>0.00729450171126801</v>
+      </c>
+      <c r="U95" t="n">
+        <v>81.9783041491569</v>
       </c>
     </row>
     <row r="96">
@@ -7280,15 +7478,17 @@
       <c r="Q96" t="n">
         <v>0.0008890854041372103</v>
       </c>
-      <c r="R96" t="inlineStr">
-        <is>
-          <t>[0.00315583]</t>
-        </is>
-      </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>[82.86657251]</t>
-        </is>
+      <c r="R96" t="n">
+        <v>0.003155830567605923</v>
+      </c>
+      <c r="S96" t="n">
+        <v>82.86657250825829</v>
+      </c>
+      <c r="T96" t="n">
+        <v>0.005254134791008711</v>
+      </c>
+      <c r="U96" t="n">
+        <v>83.61551667354649</v>
       </c>
     </row>
     <row r="97">
@@ -7351,15 +7551,17 @@
       <c r="Q97" t="n">
         <v>-0.000222000120179656</v>
       </c>
-      <c r="R97" t="inlineStr">
-        <is>
-          <t>[0.0037197]</t>
-        </is>
-      </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>[75.17641343]</t>
-        </is>
+      <c r="R97" t="n">
+        <v>0.00371970328915479</v>
+      </c>
+      <c r="S97" t="n">
+        <v>75.1764134278813</v>
+      </c>
+      <c r="T97" t="n">
+        <v>0.009032348095043243</v>
+      </c>
+      <c r="U97" t="n">
+        <v>78.50999369981329</v>
       </c>
     </row>
     <row r="98">
@@ -7422,15 +7624,17 @@
       <c r="Q98" t="n">
         <v>0.002770838845663657</v>
       </c>
-      <c r="R98" t="inlineStr">
-        <is>
-          <t>[0.00366839]</t>
-        </is>
-      </c>
-      <c r="S98" t="inlineStr">
-        <is>
-          <t>[79.8920284]</t>
-        </is>
+      <c r="R98" t="n">
+        <v>0.003668388214462446</v>
+      </c>
+      <c r="S98" t="n">
+        <v>79.89202840394329</v>
+      </c>
+      <c r="T98" t="n">
+        <v>0.007558006757768757</v>
+      </c>
+      <c r="U98" t="n">
+        <v>82.1477498523379</v>
       </c>
     </row>
     <row r="99">
@@ -7493,15 +7697,17 @@
       <c r="Q99" t="n">
         <v>0.001264873486175366</v>
       </c>
-      <c r="R99" t="inlineStr">
-        <is>
-          <t>[0.00559269]</t>
-        </is>
-      </c>
-      <c r="S99" t="inlineStr">
-        <is>
-          <t>[87.23453043]</t>
-        </is>
+      <c r="R99" t="n">
+        <v>0.005592694443305021</v>
+      </c>
+      <c r="S99" t="n">
+        <v>87.23453042602983</v>
+      </c>
+      <c r="T99" t="n">
+        <v>0.007277652320397766</v>
+      </c>
+      <c r="U99" t="n">
+        <v>87.7212251518954</v>
       </c>
     </row>
     <row r="100">
@@ -7568,15 +7774,17 @@
       <c r="Q100" t="n">
         <v>0.001600669794872614</v>
       </c>
-      <c r="R100" t="inlineStr">
-        <is>
-          <t>[0.00581256]</t>
-        </is>
-      </c>
-      <c r="S100" t="inlineStr">
-        <is>
-          <t>[88.79472099]</t>
-        </is>
+      <c r="R100" t="n">
+        <v>0.005812557635492952</v>
+      </c>
+      <c r="S100" t="n">
+        <v>88.79472099454641</v>
+      </c>
+      <c r="T100" t="n">
+        <v>0.01010092047234112</v>
+      </c>
+      <c r="U100" t="n">
+        <v>89.9980012086873</v>
       </c>
     </row>
     <row r="101">
@@ -7639,15 +7847,17 @@
       <c r="Q101" t="n">
         <v>0.0006138388323634388</v>
       </c>
-      <c r="R101" t="inlineStr">
-        <is>
-          <t>[0.00479692]</t>
-        </is>
-      </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>[92.92190035]</t>
-        </is>
+      <c r="R101" t="n">
+        <v>0.004796916024405892</v>
+      </c>
+      <c r="S101" t="n">
+        <v>92.92190034505387</v>
+      </c>
+      <c r="T101" t="n">
+        <v>0.006358843587689939</v>
+      </c>
+      <c r="U101" t="n">
+        <v>93.3946774514764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>